<commit_message>
Poprawki w zdaniach z rekcja. Dodane slownictwo z banku.
</commit_message>
<xml_diff>
--- a/nv-verbindungen/n-v-ver-sätze.xlsx
+++ b/nv-verbindungen/n-v-ver-sätze.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Das machte auf mich einen großen Eindruck.</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Jestem bardzo zadowolony ze swojego osiągnięcia.</t>
+  </si>
+  <si>
+    <t>Er hat Angst vor Hunden.</t>
+  </si>
+  <si>
+    <t>On boi się psów. (A)</t>
   </si>
 </sst>
 </file>
@@ -147,37 +153,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -475,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A17" sqref="A17:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -621,6 +630,14 @@
       </c>
       <c r="C16" s="16" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="41.4">
+      <c r="A17" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>